<commit_message>
recategorized care & support from mission to unrestricted
</commit_message>
<xml_diff>
--- a/input_files/map.xlsx
+++ b/input_files/map.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\01_Dave\Programs\GitHub_home\budget_compare\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A410EA60-B478-4BD0-BEA5-CA3C0EE39934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63D4BF00-489B-4DB5-A4F0-DA883EC7C281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1703,10 +1703,10 @@
   </sheetPr>
   <dimension ref="A1:O230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L17" sqref="L17"/>
-      <selection pane="bottomLeft" activeCell="H220" sqref="H220"/>
+      <selection pane="bottomLeft" activeCell="G139" sqref="G127:G139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8031,8 +8031,8 @@
       <c r="F127" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G127" s="4" t="s">
-        <v>13</v>
+      <c r="G127" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="H127" s="1" t="s">
         <v>95</v>
@@ -8081,8 +8081,8 @@
       <c r="F128" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G128" s="4" t="s">
-        <v>13</v>
+      <c r="G128" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="H128" s="1" t="s">
         <v>96</v>
@@ -8131,8 +8131,8 @@
       <c r="F129" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G129" s="4" t="s">
-        <v>13</v>
+      <c r="G129" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="H129" s="1" t="s">
         <v>97</v>
@@ -8181,8 +8181,8 @@
       <c r="F130" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G130" s="4" t="s">
-        <v>13</v>
+      <c r="G130" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="H130" s="1" t="s">
         <v>98</v>
@@ -8231,8 +8231,8 @@
       <c r="F131" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G131" s="4" t="s">
-        <v>13</v>
+      <c r="G131" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="H131" s="1" t="s">
         <v>99</v>
@@ -8281,8 +8281,8 @@
       <c r="F132" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G132" s="4" t="s">
-        <v>13</v>
+      <c r="G132" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="H132" s="1" t="s">
         <v>100</v>
@@ -8331,8 +8331,8 @@
       <c r="F133" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G133" s="4" t="s">
-        <v>13</v>
+      <c r="G133" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="H133" s="1" t="s">
         <v>101</v>
@@ -8381,8 +8381,8 @@
       <c r="F134" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G134" s="4" t="s">
-        <v>13</v>
+      <c r="G134" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="H134" s="1" t="s">
         <v>102</v>
@@ -8431,8 +8431,8 @@
       <c r="F135" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="G135" s="4" t="s">
-        <v>13</v>
+      <c r="G135" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="H135" s="1" t="s">
         <v>89</v>
@@ -8481,8 +8481,8 @@
       <c r="F136" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="G136" s="4" t="s">
-        <v>13</v>
+      <c r="G136" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="H136" s="1" t="s">
         <v>91</v>
@@ -8531,8 +8531,8 @@
       <c r="F137" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="G137" s="4" t="s">
-        <v>13</v>
+      <c r="G137" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="H137" s="1" t="s">
         <v>92</v>
@@ -8581,8 +8581,8 @@
       <c r="F138" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="G138" s="4" t="s">
-        <v>13</v>
+      <c r="G138" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="H138" s="1" t="s">
         <v>93</v>
@@ -8631,8 +8631,8 @@
       <c r="F139" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="G139" s="4" t="s">
-        <v>13</v>
+      <c r="G139" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="H139" s="1" t="s">
         <v>94</v>
@@ -8881,8 +8881,8 @@
       <c r="F144" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="G144" s="1" t="s">
-        <v>3</v>
+      <c r="G144" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="H144" s="1" t="s">
         <v>108</v>
@@ -8931,8 +8931,8 @@
       <c r="F145" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="G145" s="1" t="s">
-        <v>3</v>
+      <c r="G145" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="H145" s="1" t="s">
         <v>110</v>
@@ -8981,8 +8981,8 @@
       <c r="F146" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="G146" s="1" t="s">
-        <v>3</v>
+      <c r="G146" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="H146" s="1" t="s">
         <v>111</v>
@@ -9031,8 +9031,8 @@
       <c r="F147" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="G147" s="1" t="s">
-        <v>3</v>
+      <c r="G147" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="H147" s="1" t="s">
         <v>112</v>
@@ -13205,7 +13205,7 @@
   </sheetData>
   <autoFilter ref="A1:O233" xr:uid="{9210D030-08A6-47C5-BE1B-A368CD904E6C}"/>
   <conditionalFormatting sqref="A2:O9999">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>MOD($O2,2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23309,7 +23309,7 @@
   </sheetData>
   <autoFilter ref="A1:N232" xr:uid="{9210D030-08A6-47C5-BE1B-A368CD904E6C}"/>
   <conditionalFormatting sqref="A2:N2 A3:H221 J3:N221 I3:I229 A222:A229">
-    <cfRule type="expression" dxfId="2" priority="5">
+    <cfRule type="expression" dxfId="1" priority="5">
       <formula>MOD($N2,2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23840,7 +23840,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:M14">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD($M1,2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>